<commit_message>
Se añaden costes de mantenimiento #1
</commit_message>
<xml_diff>
--- a/DRS/presupuesto2.xlsx
+++ b/DRS/presupuesto2.xlsx
@@ -1,30 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Máster-Visión Artificial\2O-CUATRI\1-Aplicaciones Industriales y Comerciales\Proyecto_Deteccion_Arboles\AIVA_2021-imagenes_aereas\DRS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MUVA\2-trimestre\aplicaciones_industriales_y_comerciales\AIVA_2021-imagenes_aereas\DRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6447B1C3-4C28-4046-83F9-11492AA2EF24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="5550" yWindow="2250" windowWidth="23880" windowHeight="12990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Desarrollo Proyecto" sheetId="1" r:id="rId1"/>
+    <sheet name="Mantenimiento" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <r>
       <rPr>
@@ -154,14 +165,20 @@
   <si>
     <t>Presupuesto del proyecto: Detección de árboles en imágenes aéreas</t>
   </si>
+  <si>
+    <t>Mantenimiento</t>
+  </si>
+  <si>
+    <t>Disponivilidad y mantenimiento de los servidores (por mes)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -305,21 +322,15 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,7 +341,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -341,7 +352,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -622,11 +639,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,46 +657,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -687,211 +704,211 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F5" s="3"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>75</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <f>D8*C8</f>
         <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>150</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <f>D9*C9</f>
         <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="8" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <f>E8+E9</f>
         <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>2</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>1500</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="13">
         <v>6000</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="8" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="14">
         <f>E13</f>
         <v>6000</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="4">
         <v>1</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>250</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <f>D17*C17</f>
         <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <v>450</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <f t="shared" ref="E18:E19" si="0">D18*C18</f>
         <v>450</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <v>300</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="17" t="s">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <f>E17+E18+E19</f>
         <v>1000</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="19">
         <f>E20+E14+E10</f>
         <v>7225</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="19">
         <f>E21*1.21</f>
         <v>8742.25</v>
       </c>
@@ -905,4 +922,98 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768D1679-93D0-45A6-94F6-82E4D1D16174}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E3" s="5">
+        <f>D3*C3</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7">
+        <f>E3</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="19">
+        <f>E4</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="19">
+        <f>E5*1.21</f>
+        <v>3025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>